<commit_message>
Added "block" to the script for SUA vs NTNU soil methods, and updated the graphs.
</commit_message>
<xml_diff>
--- a/Termites/Soil data/Soil_texture.xlsx
+++ b/Termites/Soil data/Soil_texture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansun\Documents\Master data\GitHub__R-stat\AfricanBioServices-Vegetation-and-soils\Termites\Soil data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C88CB93-5BB1-4D18-BC2C-B061ED59A6FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2A198E38-9BA1-4883-BBF6-D96B2FC49199}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{2FAB7891-ACAD-4DA8-970A-DA16DFF324A3}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="29">
   <si>
     <t>sandy clay loam</t>
-  </si>
-  <si>
-    <t>Average common garden</t>
   </si>
   <si>
     <t>sandy loam</t>
@@ -121,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -134,11 +131,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
@@ -163,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -175,10 +167,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384A14F9-9808-4C47-8E0F-BB3D2EAF5BB9}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -511,55 +499,52 @@
     <col min="4" max="4" width="20.88671875" customWidth="1"/>
     <col min="6" max="6" width="14.109375" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.8">
+    <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="J1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="2" spans="1:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
@@ -585,18 +570,16 @@
       <c r="K2" s="2">
         <v>1.2493839329719072</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4">
         <v>3</v>
@@ -617,23 +600,21 @@
         <v>75.12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2">
         <v>1.641498275012321</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13">
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -659,18 +640,16 @@
       <c r="K4" s="2">
         <v>1.7491375061606702</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13">
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4">
         <v>4</v>
@@ -696,18 +675,16 @@
       <c r="K5" s="2">
         <v>1.7568260226712666</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -728,23 +705,21 @@
         <v>86.467745324648035</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="2">
         <v>1.0225726959093147</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4">
         <v>2</v>
@@ -770,18 +745,16 @@
       <c r="K7" s="2">
         <v>0.46131099063578063</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13">
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4">
         <v>3</v>
@@ -802,23 +775,21 @@
         <v>24.654545441741845</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" s="2">
         <v>1.8433218334154755</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13">
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
@@ -839,23 +810,21 @@
         <v>29.120000000000005</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" s="2">
         <v>1.85293247905372</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13">
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
@@ -876,23 +845,21 @@
         <v>29.120000000000012</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K10" s="2">
         <v>2.8831936914736325</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13">
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -913,23 +880,21 @@
         <v>31.122554067971166</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K11" s="2">
         <v>2.0547560374568752</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13">
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -950,23 +915,21 @@
         <v>34.495373359156439</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" s="2">
         <v>2.5483587974371611</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13">
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -992,18 +955,16 @@
       <c r="K13" s="2">
         <v>2.1716214884179394</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13">
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1029,18 +990,16 @@
       <c r="K14" s="2">
         <v>1.7337604731394776</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13">
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
@@ -1066,18 +1025,16 @@
       <c r="K15" s="2">
         <v>2.072055199605717</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13">
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="4">
         <v>2</v>
@@ -1098,23 +1055,21 @@
         <v>47.12</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K16" s="2">
         <v>1.6549531789058647</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13">
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
@@ -1140,18 +1095,16 @@
       <c r="K17" s="2">
         <v>1.0437161163134547</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13">
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1172,23 +1125,21 @@
         <v>39.119999999999997</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K18" s="2">
         <v>2.0374568753080333</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13">
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
@@ -1214,18 +1165,16 @@
       <c r="K19" s="2">
         <v>1.7452932479053718</v>
       </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13">
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="4">
         <v>3</v>
@@ -1251,18 +1200,16 @@
       <c r="K20" s="2">
         <v>0.88610152784622953</v>
       </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13">
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
@@ -1283,23 +1230,21 @@
         <v>77.12</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
         <v>2.0220798422868409</v>
       </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13">
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -1325,18 +1270,16 @@
       <c r="K22" s="2">
         <v>1.2416954164613114</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13">
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="4">
         <v>4</v>
@@ -1362,18 +1305,16 @@
       <c r="K23" s="2">
         <v>3.30913750616067</v>
       </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13">
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -1399,18 +1340,16 @@
       <c r="K24" s="2">
         <v>1.614588467225234</v>
       </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13">
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
@@ -1436,18 +1375,16 @@
       <c r="K25" s="2">
         <v>1.6991621488417901</v>
       </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13">
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -1474,15 +1411,15 @@
         <v>1.0994578610152781</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:11">
       <c r="A27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
@@ -1509,15 +1446,15 @@
         <v>1.4512074913750617</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:11">
       <c r="A28" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="4">
         <v>3</v>
@@ -1544,15 +1481,15 @@
         <v>1.4012321340561851</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:11">
       <c r="A29" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="4">
         <v>4</v>
@@ -1573,52 +1510,11 @@
         <v>77.11999999999999</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2">
         <v>0.60547067520946207</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="2">
-        <f>AVERAGE(G26:G29)</f>
-        <v>22.017293559158162</v>
-      </c>
-      <c r="H30" s="2">
-        <f>AVERAGE(H26:H29)</f>
-        <v>6.5855206693798616</v>
-      </c>
-      <c r="I30" s="2">
-        <f>AVERAGE(I26:I29)</f>
-        <v>71.397185771461977</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K30" s="5">
-        <f>AVERAGE(K26:K29)</f>
-        <v>1.1393420404139967</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>